<commit_message>
ADD: atualização excel e adição de funções pytest
</commit_message>
<xml_diff>
--- a/casos_teste_juros.xlsx
+++ b/casos_teste_juros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENAI\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\OneDrive\Área de Trabalho\juros_compostos_pytest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37DA0CA-3923-408F-8225-3819A92601DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B7E188-D3F2-4CC1-98B5-C10F8968377D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{986F6839-49ED-4DD7-8217-0C19B97974F9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{986F6839-49ED-4DD7-8217-0C19B97974F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -69,15 +69,9 @@
     <t>Verifica se é string</t>
   </si>
   <si>
-    <t>"oi"</t>
-  </si>
-  <si>
     <t>Verifica se os parâmetros estão vazios</t>
   </si>
   <si>
-    <t>""</t>
-  </si>
-  <si>
     <t>Verifica string com int/float</t>
   </si>
   <si>
@@ -90,9 +84,6 @@
     <t>[1000, 20, 1]</t>
   </si>
   <si>
-    <t>[-1000, 20, 1]</t>
-  </si>
-  <si>
     <t>ValueError: ("Apenas valores positivos")</t>
   </si>
   <si>
@@ -109,6 +100,15 @@
   </si>
   <si>
     <t>ValueError: ("Apenas duas casas decimais")</t>
+  </si>
+  <si>
+    <t>[-1000, -20, -1]</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>"str"</t>
   </si>
 </sst>
 </file>
@@ -425,13 +425,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -448,6 +441,13 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -492,7 +492,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78953D28-7E6F-442A-9A58-A2D4206F942E}" name="Tabela1" displayName="Tabela1" ref="B2:F13" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{78953D28-7E6F-442A-9A58-A2D4206F942E}" name="Tabela1" displayName="Tabela1" ref="B2:F13" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
   <autoFilter ref="B2:F13" xr:uid="{B384DCA7-400A-43B1-9A15-843DA3BA9D12}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{E79A1A6A-2F40-43AF-B449-E1D504DF3763}" name="ARQUIVOS" dataDxfId="4"/>
@@ -805,7 +805,7 @@
   <dimension ref="B2:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -849,7 +849,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F3" s="9">
         <v>1200</v>
@@ -869,10 +869,10 @@
         <v>8</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>10</v>
@@ -889,10 +889,10 @@
         <v>13</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H5" s="15" t="s">
         <v>11</v>
@@ -906,13 +906,13 @@
         <v>7</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -923,13 +923,13 @@
         <v>7</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -940,13 +940,13 @@
         <v>7</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
MODIFY: ajustes gerais excel funções
</commit_message>
<xml_diff>
--- a/casos_teste_juros.xlsx
+++ b/casos_teste_juros.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20343"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\OneDrive\Área de Trabalho\juros_compostos_pytest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENAI\Desktop\juros_compostos_pytest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B7E188-D3F2-4CC1-98B5-C10F8968377D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C98AEC-2180-4055-B0C7-AAD0C9662A6E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{986F6839-49ED-4DD7-8217-0C19B97974F9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
   <si>
     <t>ARQUIVOS</t>
   </si>
@@ -66,18 +66,12 @@
     <t>parâmetros:</t>
   </si>
   <si>
-    <t>Verifica se é string</t>
-  </si>
-  <si>
     <t>Verifica se os parâmetros estão vazios</t>
   </si>
   <si>
     <t>Verifica string com int/float</t>
   </si>
   <si>
-    <t>Verifica/corrige as casas decimais(apenas duas casas)</t>
-  </si>
-  <si>
     <t>ValueError: ("valores vazios")</t>
   </si>
   <si>
@@ -90,25 +84,25 @@
     <t>TypeError: ("Apenas números")</t>
   </si>
   <si>
-    <t>["oi", 20, 1]</t>
-  </si>
-  <si>
-    <t>ValueError: ("valor com string")</t>
-  </si>
-  <si>
-    <t>[1000, 25.555, 1.234]</t>
-  </si>
-  <si>
-    <t>ValueError: ("Apenas duas casas decimais")</t>
-  </si>
-  <si>
-    <t>[-1000, -20, -1]</t>
-  </si>
-  <si>
     <t>[]</t>
   </si>
   <si>
-    <t>"str"</t>
+    <t>["str", 20, 1]</t>
+  </si>
+  <si>
+    <t>[-1000, 20, 1]</t>
+  </si>
+  <si>
+    <t>[1000, -20, 1]</t>
+  </si>
+  <si>
+    <t>[1000, 20, -1]</t>
+  </si>
+  <si>
+    <t>[1000, "str", 1]</t>
+  </si>
+  <si>
+    <t>[1000, 20, "str"]</t>
   </si>
 </sst>
 </file>
@@ -145,7 +139,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -257,17 +251,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -279,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -314,12 +297,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -805,7 +791,7 @@
   <dimension ref="B2:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -834,7 +820,7 @@
       <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="12" t="s">
         <v>12</v>
       </c>
     </row>
@@ -849,12 +835,12 @@
         <v>5</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F3" s="9">
         <v>1200</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="13" t="s">
         <v>9</v>
       </c>
     </row>
@@ -869,12 +855,12 @@
         <v>8</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="13" t="s">
         <v>10</v>
       </c>
     </row>
@@ -886,15 +872,15 @@
         <v>7</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="14" t="s">
         <v>11</v>
       </c>
     </row>
@@ -906,10 +892,10 @@
         <v>7</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>17</v>
@@ -923,13 +909,13 @@
         <v>7</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -939,14 +925,14 @@
       <c r="C8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="6" t="s">
+      <c r="D8" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="15" t="s">
         <v>24</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -956,9 +942,15 @@
       <c r="C9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="9"/>
+      <c r="D9" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="10" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
@@ -967,9 +959,15 @@
       <c r="C10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="6"/>
+      <c r="D10" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="11" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
@@ -989,9 +987,9 @@
       <c r="C12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="6"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="16"/>
     </row>
     <row r="13" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
@@ -1000,14 +998,15 @@
       <c r="C13" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="12"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>